<commit_message>
Updated questions and excel sheet
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>championPoints</t>
   </si>
@@ -31,6 +31,60 @@
   </si>
   <si>
     <t>championId</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>score/top3</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D-</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>S-</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S+</t>
   </si>
 </sst>
 </file>
@@ -399,31 +453,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="5" spans="1:13">
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="L11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13">
+      <c r="L17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13">
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data.xlsx and game.html script variables
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>championId</t>
   </si>
@@ -53,6 +53,9 @@
     <t>Average Score</t>
   </si>
   <si>
+    <t>Average Top3Score</t>
+  </si>
+  <si>
     <t>Average Top3Score/Score</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
   </si>
   <si>
     <t>Champion w/ Least Levels</t>
+  </si>
+  <si>
+    <t>Champion w/ Most Points</t>
   </si>
   <si>
     <t>Champion w/ Least Points</t>
@@ -135,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -157,12 +163,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,7 +212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,7 +236,7 @@
   <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -316,7 +316,7 @@
         <v>91</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1618</v>
@@ -337,7 +337,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>9204</v>
@@ -357,13 +357,21 @@
         <v>157</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>590</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">COUNTA(B3:B55)</f>
+        <v>53</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">E5/E3</f>
+        <v>0.392592592592593</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>7</v>
@@ -386,6 +394,14 @@
       <c r="D6" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">COUNTA(B56:B67)</f>
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">E6/E3</f>
+        <v>0.0888888888888889</v>
+      </c>
       <c r="G6" s="0" t="n">
         <v>54</v>
       </c>
@@ -405,13 +421,21 @@
         <v>122</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15050</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">COUNTA(B68:B86)</f>
+        <v>19</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">E7/E3</f>
+        <v>0.140740740740741</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>9</v>
@@ -426,13 +450,21 @@
         <v>78</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2311</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">COUNTA(B87:B113)</f>
+        <v>27</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">E8/E3</f>
+        <v>0.2</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>5</v>
@@ -453,13 +485,21 @@
         <v>245</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1125</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">COUNTA(B114:B138)</f>
+        <v>25</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">E9/E3</f>
+        <v>0.185185185185185</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>11</v>
@@ -474,7 +514,7 @@
         <v>412</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>5881</v>
@@ -489,8 +529,8 @@
         <v>12</v>
       </c>
       <c r="L10" s="0" t="n">
-        <f aca="false">H2/G2</f>
-        <v>0.152082076041038</v>
+        <f aca="false">H2/F2</f>
+        <v>10.08</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,13 +538,17 @@
         <v>111</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1201</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">H2/G2</f>
+        <v>0.152082076041038</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,7 +556,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>17856</v>
@@ -528,6 +572,9 @@
       </c>
       <c r="K12" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>412</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +582,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>16022</v>
@@ -545,6 +592,9 @@
       </c>
       <c r="K13" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,7 +602,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>14484</v>
@@ -562,6 +612,9 @@
       </c>
       <c r="K14" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,13 +639,16 @@
       <c r="K15" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>69</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>13816</v>
@@ -602,6 +658,9 @@
       </c>
       <c r="K16" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>0.39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +668,7 @@
         <v>223</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>12627</v>
@@ -619,6 +678,9 @@
       </c>
       <c r="K17" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>0.09</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,7 +688,7 @@
         <v>89</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2116</v>
@@ -642,6 +704,9 @@
       </c>
       <c r="K18" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>0.14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,13 +714,19 @@
         <v>67</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1466</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +734,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1449</v>
@@ -671,13 +742,19 @@
       <c r="D20" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="K20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1147</v>
@@ -697,7 +774,7 @@
         <v>103</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1356</v>
@@ -714,7 +791,7 @@
         <v>92</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1084</v>
@@ -725,7 +802,7 @@
         <v>81</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>200</v>
@@ -784,7 +861,7 @@
         <v>412</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>4781</v>
@@ -801,7 +878,7 @@
         <v>80</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>4303</v>
@@ -812,7 +889,7 @@
         <v>103</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>4298</v>
@@ -823,7 +900,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2507</v>
@@ -840,7 +917,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>1384</v>
@@ -851,7 +928,7 @@
         <v>78</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>7026</v>
@@ -871,7 +948,7 @@
         <v>64</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>6901</v>
@@ -885,7 +962,7 @@
         <v>412</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>5024</v>
@@ -896,7 +973,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>7181</v>
@@ -913,7 +990,7 @@
         <v>267</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>1873</v>
@@ -924,7 +1001,7 @@
         <v>103</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1288</v>
@@ -935,7 +1012,7 @@
         <v>54</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>5188</v>
@@ -952,7 +1029,7 @@
         <v>67</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>170</v>
@@ -963,7 +1040,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>147</v>
@@ -974,7 +1051,7 @@
         <v>102</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>11624</v>
@@ -991,7 +1068,7 @@
         <v>133</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>173</v>
@@ -1067,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>11953</v>
@@ -1078,7 +1155,7 @@
         <v>92</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>2696</v>
@@ -1176,7 +1253,7 @@
         <v>161</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>50111</v>
@@ -1215,7 +1292,7 @@
         <v>412</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>32538</v>
@@ -1235,7 +1312,7 @@
         <v>429</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>22513</v>
@@ -1263,7 +1340,7 @@
         <v>105</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>258</v>
@@ -1280,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>10240</v>
@@ -1300,7 +1377,7 @@
         <v>67</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>5278</v>
@@ -1314,7 +1391,7 @@
         <v>99</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>3448</v>
@@ -1328,7 +1405,7 @@
         <v>48</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>4240</v>
@@ -1345,7 +1422,7 @@
         <v>89</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>2970</v>
@@ -1356,7 +1433,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>2856</v>
@@ -1367,7 +1444,7 @@
         <v>25</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>20091</v>
@@ -1384,7 +1461,7 @@
         <v>412</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>4257</v>
@@ -1395,7 +1472,7 @@
         <v>421</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>3005</v>
@@ -1406,7 +1483,7 @@
         <v>92</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>48506</v>
@@ -1454,7 +1531,7 @@
         <v>22</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>329</v>
@@ -1527,7 +1604,7 @@
         <v>19</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>5132</v>
@@ -1538,7 +1615,7 @@
         <v>23</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>2007</v>
@@ -1549,7 +1626,7 @@
         <v>22</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>1184</v>
@@ -1566,7 +1643,7 @@
         <v>40</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>1075</v>
@@ -1577,7 +1654,7 @@
         <v>37</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>874</v>
@@ -1588,7 +1665,7 @@
         <v>143</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>183676</v>
@@ -1608,7 +1685,7 @@
         <v>40</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>83027</v>
@@ -1622,7 +1699,7 @@
         <v>39</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>71634</v>
@@ -1675,7 +1752,7 @@
         <v>117</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>9417</v>
@@ -1695,7 +1772,7 @@
         <v>12</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>7654</v>
@@ -1706,7 +1783,7 @@
         <v>412</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>6861</v>
@@ -1717,7 +1794,7 @@
         <v>131</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>49187</v>
@@ -1734,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>37431</v>
@@ -1748,7 +1825,7 @@
         <v>114</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>36120</v>
@@ -1762,7 +1839,7 @@
         <v>238</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>39498</v>
@@ -1782,7 +1859,7 @@
         <v>67</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C98" s="0" t="n">
         <v>32251</v>
@@ -1793,7 +1870,7 @@
         <v>254</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>25557</v>
@@ -1807,7 +1884,7 @@
         <v>69</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>1797</v>
@@ -1824,13 +1901,13 @@
         <v>114</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>1619</v>
       </c>
       <c r="L101" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M101" s="0" t="n">
         <v>1</v>
@@ -1841,13 +1918,13 @@
         <v>64</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>1609</v>
       </c>
       <c r="L102" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M102" s="0" t="n">
         <v>2</v>
@@ -1858,7 +1935,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>46343</v>
@@ -1873,7 +1950,7 @@
         <v>15</v>
       </c>
       <c r="L103" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M103" s="0" t="n">
         <v>3</v>
@@ -1884,7 +1961,7 @@
         <v>236</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>43835</v>
@@ -1893,7 +1970,7 @@
         <v>15</v>
       </c>
       <c r="L104" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M104" s="0" t="n">
         <v>4</v>
@@ -1904,7 +1981,7 @@
         <v>15</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C105" s="0" t="n">
         <v>27208</v>
@@ -1913,7 +1990,7 @@
         <v>11</v>
       </c>
       <c r="L105" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M105" s="0" t="n">
         <v>5</v>
@@ -1924,7 +2001,7 @@
         <v>412</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>61081</v>
@@ -1939,7 +2016,7 @@
         <v>14</v>
       </c>
       <c r="L106" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M106" s="0" t="n">
         <v>6</v>
@@ -1950,7 +2027,7 @@
         <v>12</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>25374</v>
@@ -1959,7 +2036,7 @@
         <v>15</v>
       </c>
       <c r="L107" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M107" s="0" t="n">
         <v>7</v>
@@ -1970,7 +2047,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>16798</v>
@@ -1979,7 +2056,7 @@
         <v>13</v>
       </c>
       <c r="L108" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M108" s="0" t="n">
         <v>8</v>
@@ -1990,7 +2067,7 @@
         <v>53</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>41482</v>
@@ -2005,7 +2082,7 @@
         <v>15</v>
       </c>
       <c r="L109" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M109" s="0" t="n">
         <v>9</v>
@@ -2016,7 +2093,7 @@
         <v>98</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>23177</v>
@@ -2025,7 +2102,7 @@
         <v>13</v>
       </c>
       <c r="L110" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M110" s="0" t="n">
         <v>10</v>
@@ -2036,13 +2113,13 @@
         <v>90</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>22112</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M111" s="0" t="n">
         <v>11</v>
@@ -2053,7 +2130,7 @@
         <v>45</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>58728</v>
@@ -2068,7 +2145,7 @@
         <v>15</v>
       </c>
       <c r="L112" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M112" s="0" t="n">
         <v>12</v>
@@ -2079,7 +2156,7 @@
         <v>67</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>45170</v>
@@ -2088,7 +2165,7 @@
         <v>10</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M113" s="0" t="n">
         <v>13</v>
@@ -2099,7 +2176,7 @@
         <v>90</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C114" s="0" t="n">
         <v>35276</v>
@@ -2108,7 +2185,7 @@
         <v>15</v>
       </c>
       <c r="L114" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M114" s="0" t="n">
         <v>14</v>
@@ -2119,7 +2196,7 @@
         <v>89</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>2074</v>
@@ -2134,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M115" s="0" t="n">
         <v>15</v>
@@ -2154,7 +2231,7 @@
         <v>9</v>
       </c>
       <c r="L116" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M116" s="0" t="n">
         <v>16</v>
@@ -2179,7 +2256,7 @@
         <v>22</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C118" s="0" t="n">
         <v>12242</v>
@@ -2199,7 +2276,7 @@
         <v>110</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C119" s="0" t="n">
         <v>11313</v>
@@ -2213,7 +2290,7 @@
         <v>18</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C120" s="0" t="n">
         <v>9511</v>
@@ -2227,7 +2304,7 @@
         <v>236</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>30248</v>
@@ -2247,7 +2324,7 @@
         <v>42</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>24454</v>
@@ -2261,7 +2338,7 @@
         <v>81</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>19560</v>
@@ -2275,7 +2352,7 @@
         <v>236</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>47599</v>
@@ -2295,7 +2372,7 @@
         <v>429</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>41659</v>
@@ -2309,7 +2386,7 @@
         <v>202</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>33441</v>
@@ -2323,7 +2400,7 @@
         <v>107</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>144588</v>
@@ -2340,7 +2417,7 @@
         <v>60</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C128" s="0" t="n">
         <v>105705</v>
@@ -2354,7 +2431,7 @@
         <v>64</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C129" s="0" t="n">
         <v>71514</v>
@@ -2365,7 +2442,7 @@
         <v>432</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>68994</v>
@@ -2385,7 +2462,7 @@
         <v>67</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C131" s="0" t="n">
         <v>46681</v>
@@ -2396,7 +2473,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C132" s="0" t="n">
         <v>42421</v>
@@ -2410,7 +2487,7 @@
         <v>64</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C133" s="0" t="n">
         <v>66354</v>
@@ -2427,7 +2504,7 @@
         <v>7</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>65493</v>
@@ -2438,7 +2515,7 @@
         <v>268</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>52996</v>
@@ -2449,7 +2526,7 @@
         <v>15</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>3896</v>
@@ -2466,7 +2543,7 @@
         <v>51</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>2425</v>
@@ -2477,7 +2554,7 @@
         <v>81</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>1837</v>

</xml_diff>